<commit_message>
trimming data is updated
</commit_message>
<xml_diff>
--- a/inventvmScripts/effieciency/effiecincy1.xlsx
+++ b/inventvmScripts/effieciency/effiecincy1.xlsx
@@ -30,6 +30,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ph1234_vbat_4V_vbus_15V" sheetId="22" state="visible" r:id="rId22"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ph1234_ph1_vbat_4V_vbus_15V" sheetId="23" state="visible" r:id="rId23"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ph12_ph1_vbat_4V_vbus_9V_1" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="dummy" sheetId="25" state="visible" r:id="rId25"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -43865,6 +43866,579 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>vbat_V</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>ibat_A</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>vbus_V</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>ibus_A</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>efficiency</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>3.9890679875</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.1004135</v>
+      </c>
+      <c r="C2" t="n">
+        <v>9.004001000000001</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.05225086</v>
+      </c>
+      <c r="E2" t="n">
+        <v>85.14018035526433</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3.9890748275</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.100416</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9.004002</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.05227101</v>
+      </c>
+      <c r="E3" t="n">
+        <v>85.10961499425376</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.9902983525</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.2004981</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9.003961</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.09682997</v>
+      </c>
+      <c r="E4" t="n">
+        <v>91.76397708382639</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3.9918559025</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.3004653</v>
+      </c>
+      <c r="C5" t="n">
+        <v>9.003992999999999</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1416674</v>
+      </c>
+      <c r="E5" t="n">
+        <v>94.02949578439697</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>3.9936480175</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.4004739</v>
+      </c>
+      <c r="C6" t="n">
+        <v>9.003996000000001</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1866496</v>
+      </c>
+      <c r="E6" t="n">
+        <v>95.1659627777638</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3.9950499225</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.5004818</v>
+      </c>
+      <c r="C7" t="n">
+        <v>9.003871</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.2320144</v>
+      </c>
+      <c r="E7" t="n">
+        <v>95.71197881913486</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>3.996719685</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.6005057</v>
+      </c>
+      <c r="C8" t="n">
+        <v>9.003921</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.2776032</v>
+      </c>
+      <c r="E8" t="n">
+        <v>96.02065844021489</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>3.998580715</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.7005562</v>
+      </c>
+      <c r="C9" t="n">
+        <v>9.003899000000001</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.3234304</v>
+      </c>
+      <c r="E9" t="n">
+        <v>96.1916546736407</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>4.000355595</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.8005186</v>
+      </c>
+      <c r="C10" t="n">
+        <v>9.004004</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.3694859</v>
+      </c>
+      <c r="E10" t="n">
+        <v>96.25792065245291</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>4.00187433</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.9005030000000001</v>
+      </c>
+      <c r="C11" t="n">
+        <v>9.003869</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.4155703</v>
+      </c>
+      <c r="E11" t="n">
+        <v>96.3107890519925</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>4.0030724275</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1.000478</v>
+      </c>
+      <c r="C12" t="n">
+        <v>9.003776999999999</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.4620328</v>
+      </c>
+      <c r="E12" t="n">
+        <v>96.27276683247364</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>4.00497874</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1.100541</v>
+      </c>
+      <c r="C13" t="n">
+        <v>9.004151</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.5087447</v>
+      </c>
+      <c r="E13" t="n">
+        <v>96.21965030670587</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>4.00678753</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1.200615</v>
+      </c>
+      <c r="C14" t="n">
+        <v>9.004236000000001</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.5556563</v>
+      </c>
+      <c r="E14" t="n">
+        <v>96.14948589439399</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>4.0081607925</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1.300532</v>
+      </c>
+      <c r="C15" t="n">
+        <v>9.004201999999999</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.6025578</v>
+      </c>
+      <c r="E15" t="n">
+        <v>96.07761993095365</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>4.00987909</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1.400625</v>
+      </c>
+      <c r="C16" t="n">
+        <v>9.004047999999999</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.6498704</v>
+      </c>
+      <c r="E16" t="n">
+        <v>95.98173441924138</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>4.011741625</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1.500519</v>
+      </c>
+      <c r="C17" t="n">
+        <v>9.00433</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.6973712</v>
+      </c>
+      <c r="E17" t="n">
+        <v>95.86477175004329</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>4.0132960225</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1.600656</v>
+      </c>
+      <c r="C18" t="n">
+        <v>9.004076</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.7452010999999999</v>
+      </c>
+      <c r="E18" t="n">
+        <v>95.73848752412417</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>4.0152297375</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1.700475</v>
+      </c>
+      <c r="C19" t="n">
+        <v>9.004213999999999</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.7931827</v>
+      </c>
+      <c r="E19" t="n">
+        <v>95.60081817487043</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>4.016991787499999</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1.800623</v>
+      </c>
+      <c r="C20" t="n">
+        <v>9.004089</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.841364</v>
+      </c>
+      <c r="E20" t="n">
+        <v>95.47727873176729</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>4.0184857</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1.900542</v>
+      </c>
+      <c r="C21" t="n">
+        <v>9.003947</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.8897482</v>
+      </c>
+      <c r="E21" t="n">
+        <v>95.33225163876111</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>4.0200871325</v>
+      </c>
+      <c r="B22" t="n">
+        <v>2.000669</v>
+      </c>
+      <c r="C22" t="n">
+        <v>9.004134000000001</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.9384987</v>
+      </c>
+      <c r="E22" t="n">
+        <v>95.17767335401078</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>4.0217745675</v>
+      </c>
+      <c r="B23" t="n">
+        <v>2.100584</v>
+      </c>
+      <c r="C23" t="n">
+        <v>9.004168</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.9874233</v>
+      </c>
+      <c r="E23" t="n">
+        <v>95.01907891187091</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>4.02373624</v>
+      </c>
+      <c r="B24" t="n">
+        <v>2.200623</v>
+      </c>
+      <c r="C24" t="n">
+        <v>9.004177</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1.036509</v>
+      </c>
+      <c r="E24" t="n">
+        <v>94.87636806853352</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>4.025525235</v>
+      </c>
+      <c r="B25" t="n">
+        <v>2.300559</v>
+      </c>
+      <c r="C25" t="n">
+        <v>9.004118999999999</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1.085759</v>
+      </c>
+      <c r="E25" t="n">
+        <v>94.72863188166613</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>4.02685571</v>
+      </c>
+      <c r="B26" t="n">
+        <v>2.400647</v>
+      </c>
+      <c r="C26" t="n">
+        <v>9.004130999999999</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.135508</v>
+      </c>
+      <c r="E26" t="n">
+        <v>94.55018209429991</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>4.028533175</v>
+      </c>
+      <c r="B27" t="n">
+        <v>2.500538</v>
+      </c>
+      <c r="C27" t="n">
+        <v>9.004217000000001</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1.185483</v>
+      </c>
+      <c r="E27" t="n">
+        <v>94.37112228487878</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>4.03024146</v>
+      </c>
+      <c r="B28" t="n">
+        <v>2.600561</v>
+      </c>
+      <c r="C28" t="n">
+        <v>9.004092</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1.23532</v>
+      </c>
+      <c r="E28" t="n">
+        <v>94.22772701581142</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>4.0317491325</v>
+      </c>
+      <c r="B29" t="n">
+        <v>2.700638</v>
+      </c>
+      <c r="C29" t="n">
+        <v>9.004217000000001</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1.285704</v>
+      </c>
+      <c r="E29" t="n">
+        <v>94.05305949086461</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>4.0334121</v>
+      </c>
+      <c r="B30" t="n">
+        <v>2.800624</v>
+      </c>
+      <c r="C30" t="n">
+        <v>9.004341999999999</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1.336512</v>
+      </c>
+      <c r="E30" t="n">
+        <v>93.8647566743014</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>4.03513508</v>
+      </c>
+      <c r="B31" t="n">
+        <v>2.900586</v>
+      </c>
+      <c r="C31" t="n">
+        <v>9.004186000000001</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1.387176</v>
+      </c>
+      <c r="E31" t="n">
+        <v>93.7060864205001</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>4.03677894</v>
+      </c>
+      <c r="B32" t="n">
+        <v>3.000629</v>
+      </c>
+      <c r="C32" t="n">
+        <v>9.004253</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1.438235</v>
+      </c>
+      <c r="E32" t="n">
+        <v>93.53404733163352</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>